<commit_message>
changing double to BigDecimal, trying to increase coordinates-precision
</commit_message>
<xml_diff>
--- a/x_documents/analyse_positionsberechnung/Analyse_Summary.xlsx
+++ b/x_documents/analyse_positionsberechnung/Analyse_Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\beacons-project\x_documents\analyse_positionsberechnung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B4367D-D8AA-45DA-B3EA-BD606D187182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2053FB05-F6F8-4388-8594-3DD926638C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A73CB475-C6BD-4B81-AB24-2C7ED570D6BF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A73CB475-C6BD-4B81-AB24-2C7ED570D6BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="106">
   <si>
     <t>Aussreisser 1:  -&gt; gleiche Position bei beiden berechnungen (SlidingWindo/NoFiltering)</t>
   </si>
@@ -364,6 +364,27 @@
   </si>
   <si>
     <t>Quelle</t>
+  </si>
+  <si>
+    <t>changing all double-types to decimal to try to increase the precision</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Conclusions:</t>
+  </si>
+  <si>
+    <t>newTrill1 berforms best</t>
+  </si>
+  <si>
+    <t>newTrill2 calculation completely wrong</t>
+  </si>
+  <si>
+    <t>current -&gt; bad performance in this scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_&gt; no visible effect in result </t>
   </si>
 </sst>
 </file>
@@ -979,6 +1000,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>49021</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>96036</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C231FB7D-83EE-4FE1-97B6-406E968B95BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7105650" y="333375"/>
+          <a:ext cx="10002646" cy="5630061"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1281,7 +1346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB7E0E6-571F-4A26-8AA2-7720358CB485}">
   <dimension ref="B2:T88"/>
   <sheetViews>
-    <sheetView topLeftCell="D47" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="D58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K22" sqref="K22:K24"/>
     </sheetView>
   </sheetViews>
@@ -2806,10 +2871,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F760675F-578D-48B5-AF61-3703979DB191}">
-  <dimension ref="A2:K9"/>
+  <dimension ref="A2:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2896,6 +2961,37 @@
         <v>0</v>
       </c>
     </row>
+    <row r="25" spans="2:7">
+      <c r="B25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="D26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="D27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="D28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>